<commit_message>
Metadatenpflege und View Überarbeitung (Schlüssel)
</commit_message>
<xml_diff>
--- a/Metadatenpflege/Metadaten_Pflege.xlsx
+++ b/Metadatenpflege/Metadaten_Pflege.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaspe\Documents\ILF\Metadatenpflege\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88ED490-1F85-46EF-93E7-99B2561CC5CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E53364-4D5E-49A0-A3F8-F0D91E1AA2A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="754" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connection" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2583" uniqueCount="660">
   <si>
     <t>ID</t>
   </si>
@@ -2460,6 +2460,15 @@
   </si>
   <si>
     <t>preprod</t>
+  </si>
+  <si>
+    <t>EXEMPLOYEE</t>
+  </si>
+  <si>
+    <t>dbo</t>
+  </si>
+  <si>
+    <t>EXJOBHEADER</t>
   </si>
 </sst>
 </file>
@@ -4392,10 +4401,10 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4934,10 +4943,10 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4948,7 +4957,7 @@
     <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -4997,8 +5006,11 @@
       <c r="C2" s="4">
         <v>6</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>658</v>
+      </c>
       <c r="E2" s="17" t="s">
-        <v>297</v>
+        <v>657</v>
       </c>
       <c r="F2" s="3">
         <v>2</v>
@@ -5021,7 +5033,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>298</v>
+        <v>659</v>
       </c>
       <c r="F3" s="3">
         <v>2</v>
@@ -5506,10 +5518,10 @@
   </sheetPr>
   <dimension ref="A1:O328"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>